<commit_message>
NXtel client now uses the Prestel character set.
</commit_message>
<xml_diff>
--- a/docs/prestel character set.xlsx
+++ b/docs/prestel character set.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\Visual Studio 2015\Projects\NXtel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69EAB71-D0B5-4E8C-BB74-526B683A5461}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13241AC8-83F2-46C7-B1ED-C0FA1A48B57C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" xr2:uid="{4E45CEFB-9C71-41FA-8F36-CA32F2ADC803}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="74">
   <si>
     <t>ASCII</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>Teletext</t>
+  </si>
+  <si>
+    <t>Shifted</t>
   </si>
 </sst>
 </file>
@@ -293,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -307,6 +310,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -622,11 +631,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FEC36D4-E8A2-4FCB-BFF9-8DA7DDB6CAE4}">
-  <dimension ref="A1:H129"/>
+  <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F75" sqref="F75"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K95" sqref="K95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,9 +648,10 @@
     <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -666,8 +676,11 @@
       <c r="H1" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -690,7 +703,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>1</v>
@@ -708,7 +721,7 @@
         <v>0001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A67" si="3">A3+1</f>
         <v>2</v>
@@ -726,7 +739,7 @@
         <v>0010</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -744,7 +757,7 @@
         <v>0011</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -762,7 +775,7 @@
         <v>0100</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -786,7 +799,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -804,7 +817,7 @@
         <v>0110</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -822,7 +835,7 @@
         <v>0111</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -846,7 +859,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -870,7 +883,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -894,7 +907,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -918,7 +931,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -942,7 +955,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -966,7 +979,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="3"/>
         <v>14</v>
@@ -1347,7 +1360,7 @@
         <v>0001</v>
       </c>
       <c r="E35" t="str">
-        <f>CHAR(A35)</f>
+        <f t="shared" ref="E35:E66" si="4">CHAR(A35)</f>
         <v>!</v>
       </c>
       <c r="F35" t="s">
@@ -1375,7 +1388,7 @@
         <v>0010</v>
       </c>
       <c r="E36" t="str">
-        <f>CHAR(A36)</f>
+        <f t="shared" si="4"/>
         <v>"</v>
       </c>
       <c r="F36" t="s">
@@ -1403,7 +1416,7 @@
         <v>0011</v>
       </c>
       <c r="E37" t="str">
-        <f>CHAR(A37)</f>
+        <f t="shared" si="4"/>
         <v>#</v>
       </c>
       <c r="F37" t="s">
@@ -1431,7 +1444,7 @@
         <v>0100</v>
       </c>
       <c r="E38" t="str">
-        <f>CHAR(A38)</f>
+        <f t="shared" si="4"/>
         <v>$</v>
       </c>
       <c r="F38" t="s">
@@ -1459,7 +1472,7 @@
         <v>0101</v>
       </c>
       <c r="E39" t="str">
-        <f>CHAR(A39)</f>
+        <f t="shared" si="4"/>
         <v>%</v>
       </c>
       <c r="F39" t="s">
@@ -1484,7 +1497,7 @@
         <v>0110</v>
       </c>
       <c r="E40" t="str">
-        <f>CHAR(A40)</f>
+        <f t="shared" si="4"/>
         <v>&amp;</v>
       </c>
       <c r="F40" t="s">
@@ -1509,7 +1522,7 @@
         <v>0111</v>
       </c>
       <c r="E41" t="str">
-        <f>CHAR(A41)</f>
+        <f t="shared" si="4"/>
         <v>'</v>
       </c>
       <c r="F41" t="s">
@@ -1534,7 +1547,7 @@
         <v>1000</v>
       </c>
       <c r="E42" t="str">
-        <f>CHAR(A42)</f>
+        <f t="shared" si="4"/>
         <v>(</v>
       </c>
       <c r="F42" t="s">
@@ -1559,7 +1572,7 @@
         <v>1001</v>
       </c>
       <c r="E43" t="str">
-        <f>CHAR(A43)</f>
+        <f t="shared" si="4"/>
         <v>)</v>
       </c>
       <c r="F43" t="s">
@@ -1584,7 +1597,7 @@
         <v>1010</v>
       </c>
       <c r="E44" t="str">
-        <f>CHAR(A44)</f>
+        <f t="shared" si="4"/>
         <v>*</v>
       </c>
       <c r="F44" t="s">
@@ -1609,7 +1622,7 @@
         <v>1011</v>
       </c>
       <c r="E45" t="str">
-        <f>CHAR(A45)</f>
+        <f t="shared" si="4"/>
         <v>+</v>
       </c>
       <c r="F45" t="s">
@@ -1634,7 +1647,7 @@
         <v>1100</v>
       </c>
       <c r="E46" t="str">
-        <f>CHAR(A46)</f>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="F46" t="s">
@@ -1659,7 +1672,7 @@
         <v>1101</v>
       </c>
       <c r="E47" t="str">
-        <f>CHAR(A47)</f>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F47" t="s">
@@ -1684,7 +1697,7 @@
         <v>1110</v>
       </c>
       <c r="E48" t="str">
-        <f>CHAR(A48)</f>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="F48" t="s">
@@ -1709,7 +1722,7 @@
         <v>1111</v>
       </c>
       <c r="E49" t="str">
-        <f>CHAR(A49)</f>
+        <f t="shared" si="4"/>
         <v>/</v>
       </c>
       <c r="F49" t="s">
@@ -1734,7 +1747,7 @@
         <v>0000</v>
       </c>
       <c r="E50" t="str">
-        <f>CHAR(A50)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F50" t="s">
@@ -1759,7 +1772,7 @@
         <v>0001</v>
       </c>
       <c r="E51" t="str">
-        <f>CHAR(A51)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F51" t="s">
@@ -1784,7 +1797,7 @@
         <v>0010</v>
       </c>
       <c r="E52" t="str">
-        <f>CHAR(A52)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="F52" t="s">
@@ -1809,7 +1822,7 @@
         <v>0011</v>
       </c>
       <c r="E53" t="str">
-        <f>CHAR(A53)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="F53" t="s">
@@ -1834,7 +1847,7 @@
         <v>0100</v>
       </c>
       <c r="E54" t="str">
-        <f>CHAR(A54)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="F54" t="s">
@@ -1859,7 +1872,7 @@
         <v>0101</v>
       </c>
       <c r="E55" t="str">
-        <f>CHAR(A55)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="F55" t="s">
@@ -1884,7 +1897,7 @@
         <v>0110</v>
       </c>
       <c r="E56" t="str">
-        <f>CHAR(A56)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="F56" t="s">
@@ -1909,7 +1922,7 @@
         <v>0111</v>
       </c>
       <c r="E57" t="str">
-        <f>CHAR(A57)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="F57" t="s">
@@ -1934,7 +1947,7 @@
         <v>1000</v>
       </c>
       <c r="E58" t="str">
-        <f>CHAR(A58)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="F58" t="s">
@@ -1959,7 +1972,7 @@
         <v>1001</v>
       </c>
       <c r="E59" t="str">
-        <f>CHAR(A59)</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="F59" t="s">
@@ -1984,7 +1997,7 @@
         <v>1010</v>
       </c>
       <c r="E60" t="str">
-        <f>CHAR(A60)</f>
+        <f t="shared" si="4"/>
         <v>:</v>
       </c>
       <c r="F60" t="s">
@@ -2009,7 +2022,7 @@
         <v>1011</v>
       </c>
       <c r="E61" t="str">
-        <f>CHAR(A61)</f>
+        <f t="shared" si="4"/>
         <v>;</v>
       </c>
       <c r="F61" t="s">
@@ -2034,7 +2047,7 @@
         <v>1100</v>
       </c>
       <c r="E62" t="str">
-        <f>CHAR(A62)</f>
+        <f t="shared" si="4"/>
         <v>&lt;</v>
       </c>
       <c r="F62" t="s">
@@ -2059,7 +2072,7 @@
         <v>1101</v>
       </c>
       <c r="E63" t="str">
-        <f>CHAR(A63)</f>
+        <f t="shared" si="4"/>
         <v>=</v>
       </c>
       <c r="F63" t="s">
@@ -2084,14 +2097,14 @@
         <v>1110</v>
       </c>
       <c r="E64" t="str">
-        <f>CHAR(A64)</f>
+        <f t="shared" si="4"/>
         <v>&gt;</v>
       </c>
       <c r="F64" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <f t="shared" si="3"/>
         <v>63</v>
@@ -2109,14 +2122,14 @@
         <v>1111</v>
       </c>
       <c r="E65" t="str">
-        <f>CHAR(A65)</f>
+        <f t="shared" si="4"/>
         <v>?</v>
       </c>
       <c r="F65" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <f t="shared" si="3"/>
         <v>64</v>
@@ -2134,29 +2147,33 @@
         <v>0000</v>
       </c>
       <c r="E66" t="str">
-        <f>CHAR(A66)</f>
+        <f t="shared" si="4"/>
         <v>@</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" s="7" t="str">
+        <f>DEC2HEX(A66+128, 2)</f>
+        <v>C0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="B67" s="1" t="str">
-        <f t="shared" ref="B67:B129" si="4">DEC2HEX(A67, 2)</f>
+        <f t="shared" ref="B67:B129" si="5">DEC2HEX(A67, 2)</f>
         <v>41</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" ref="C67:C129" si="5">MID(DEC2BIN($A67, 8), 2, 3)</f>
+        <f t="shared" ref="C67:C129" si="6">MID(DEC2BIN($A67, 8), 2, 3)</f>
         <v>100</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" ref="D67:D129" si="6">RIGHT(DEC2BIN($A67, 8), 4)</f>
+        <f t="shared" ref="D67:D129" si="7">RIGHT(DEC2BIN($A67, 8), 4)</f>
         <v>0001</v>
       </c>
       <c r="E67" t="str">
-        <f>CHAR(A67)</f>
+        <f t="shared" ref="E67:E92" si="8">CHAR(A67)</f>
         <v>A</v>
       </c>
       <c r="F67" t="s">
@@ -2166,733 +2183,841 @@
         <f>A67-65</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67" s="7" t="str">
+        <f t="shared" ref="I67:I97" si="9">DEC2HEX(A67+128, 2)</f>
+        <v>C1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <f t="shared" ref="A68:A129" si="7">A67+1</f>
+        <f t="shared" ref="A68:A129" si="10">A67+1</f>
         <v>66</v>
       </c>
       <c r="B68" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>42</v>
       </c>
       <c r="C68" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="D68" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0010</v>
       </c>
       <c r="E68" t="str">
-        <f>CHAR(A68)</f>
+        <f t="shared" si="8"/>
         <v>B</v>
       </c>
       <c r="F68" t="s">
         <v>29</v>
       </c>
       <c r="H68" s="5">
-        <f t="shared" ref="H68:H75" si="8">A68-65</f>
+        <f t="shared" ref="H68:H75" si="11">A68-65</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>C2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>67</v>
       </c>
       <c r="B69" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>43</v>
       </c>
       <c r="C69" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="D69" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0011</v>
       </c>
       <c r="E69" t="str">
-        <f>CHAR(A69)</f>
+        <f t="shared" si="8"/>
         <v>C</v>
       </c>
       <c r="F69" t="s">
         <v>30</v>
       </c>
       <c r="H69" s="5">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="I69" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>C3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <f t="shared" si="10"/>
+        <v>68</v>
+      </c>
+      <c r="B70" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>44</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="7"/>
+        <v>0100</v>
+      </c>
+      <c r="E70" t="str">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
-        <f t="shared" si="7"/>
-        <v>68</v>
-      </c>
-      <c r="B70" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>44</v>
-      </c>
-      <c r="C70" t="str">
-        <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-      <c r="D70" t="str">
-        <f t="shared" si="6"/>
-        <v>0100</v>
-      </c>
-      <c r="E70" t="str">
-        <f>CHAR(A70)</f>
         <v>D</v>
       </c>
       <c r="F70" t="s">
         <v>31</v>
       </c>
       <c r="H70" s="5">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="I70" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>C4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <f t="shared" si="10"/>
+        <v>69</v>
+      </c>
+      <c r="B71" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>45</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="7"/>
+        <v>0101</v>
+      </c>
+      <c r="E71" t="str">
         <f t="shared" si="8"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <f t="shared" si="7"/>
-        <v>69</v>
-      </c>
-      <c r="B71" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>45</v>
-      </c>
-      <c r="C71" t="str">
-        <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-      <c r="D71" t="str">
-        <f t="shared" si="6"/>
-        <v>0101</v>
-      </c>
-      <c r="E71" t="str">
-        <f>CHAR(A71)</f>
         <v>E</v>
       </c>
       <c r="F71" t="s">
         <v>32</v>
       </c>
       <c r="H71" s="5">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="I71" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>C5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <f t="shared" si="10"/>
+        <v>70</v>
+      </c>
+      <c r="B72" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>46</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="7"/>
+        <v>0110</v>
+      </c>
+      <c r="E72" t="str">
         <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <f t="shared" si="7"/>
-        <v>70</v>
-      </c>
-      <c r="B72" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>46</v>
-      </c>
-      <c r="C72" t="str">
-        <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-      <c r="D72" t="str">
-        <f t="shared" si="6"/>
-        <v>0110</v>
-      </c>
-      <c r="E72" t="str">
-        <f>CHAR(A72)</f>
         <v>F</v>
       </c>
       <c r="F72" t="s">
         <v>33</v>
       </c>
       <c r="H72" s="5">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="I72" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>C6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <f t="shared" si="10"/>
+        <v>71</v>
+      </c>
+      <c r="B73" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>47</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="7"/>
+        <v>0111</v>
+      </c>
+      <c r="E73" t="str">
         <f t="shared" si="8"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <f t="shared" si="7"/>
-        <v>71</v>
-      </c>
-      <c r="B73" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>47</v>
-      </c>
-      <c r="C73" t="str">
-        <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-      <c r="D73" t="str">
-        <f t="shared" si="6"/>
-        <v>0111</v>
-      </c>
-      <c r="E73" t="str">
-        <f>CHAR(A73)</f>
         <v>G</v>
       </c>
       <c r="F73" t="s">
         <v>34</v>
       </c>
       <c r="H73" s="5">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="I73" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>C7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <f t="shared" si="10"/>
+        <v>72</v>
+      </c>
+      <c r="B74" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="7"/>
+        <v>1000</v>
+      </c>
+      <c r="E74" t="str">
         <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <f t="shared" si="7"/>
-        <v>72</v>
-      </c>
-      <c r="B74" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>48</v>
-      </c>
-      <c r="C74" t="str">
-        <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-      <c r="D74" t="str">
-        <f t="shared" si="6"/>
-        <v>1000</v>
-      </c>
-      <c r="E74" t="str">
-        <f>CHAR(A74)</f>
         <v>H</v>
       </c>
       <c r="F74" t="s">
         <v>35</v>
       </c>
       <c r="H74" s="5">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+      <c r="I74" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>C8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <f t="shared" si="10"/>
+        <v>73</v>
+      </c>
+      <c r="B75" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>49</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="7"/>
+        <v>1001</v>
+      </c>
+      <c r="E75" t="str">
         <f t="shared" si="8"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
-        <f t="shared" si="7"/>
-        <v>73</v>
-      </c>
-      <c r="B75" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>49</v>
-      </c>
-      <c r="C75" t="str">
-        <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-      <c r="D75" t="str">
-        <f t="shared" si="6"/>
-        <v>1001</v>
-      </c>
-      <c r="E75" t="str">
-        <f>CHAR(A75)</f>
         <v>I</v>
       </c>
       <c r="F75" t="s">
         <v>36</v>
       </c>
       <c r="H75" s="5">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="I75" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>C9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <f t="shared" si="10"/>
+        <v>74</v>
+      </c>
+      <c r="B76" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>4A</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="7"/>
+        <v>1010</v>
+      </c>
+      <c r="E76" t="str">
         <f t="shared" si="8"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <f t="shared" si="7"/>
-        <v>74</v>
-      </c>
-      <c r="B76" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>4A</v>
-      </c>
-      <c r="C76" t="str">
-        <f t="shared" si="5"/>
+        <v>J</v>
+      </c>
+      <c r="I76" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>CA</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <f t="shared" si="10"/>
+        <v>75</v>
+      </c>
+      <c r="B77" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>4B</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
-      <c r="D76" t="str">
-        <f t="shared" si="6"/>
-        <v>1010</v>
-      </c>
-      <c r="E76" t="str">
-        <f>CHAR(A76)</f>
-        <v>J</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <f t="shared" si="7"/>
-        <v>75</v>
-      </c>
-      <c r="B77" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>4B</v>
-      </c>
-      <c r="C77" t="str">
-        <f t="shared" si="5"/>
+      <c r="D77" t="str">
+        <f t="shared" si="7"/>
+        <v>1011</v>
+      </c>
+      <c r="E77" t="str">
+        <f t="shared" si="8"/>
+        <v>K</v>
+      </c>
+      <c r="I77" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>CB</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <f t="shared" si="10"/>
+        <v>76</v>
+      </c>
+      <c r="B78" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>4C</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
-      <c r="D77" t="str">
-        <f t="shared" si="6"/>
-        <v>1011</v>
-      </c>
-      <c r="E77" t="str">
-        <f>CHAR(A77)</f>
-        <v>K</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <f t="shared" si="7"/>
-        <v>76</v>
-      </c>
-      <c r="B78" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>4C</v>
-      </c>
-      <c r="C78" t="str">
-        <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
       <c r="D78" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1100</v>
       </c>
       <c r="E78" t="str">
-        <f>CHAR(A78)</f>
+        <f t="shared" si="8"/>
         <v>L</v>
       </c>
       <c r="F78" t="s">
         <v>37</v>
       </c>
       <c r="H78" s="5">
-        <f t="shared" ref="H78:H79" si="9">A78-65</f>
+        <f t="shared" ref="H78:H79" si="12">A78-65</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>CC</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>77</v>
       </c>
       <c r="B79" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4D</v>
       </c>
       <c r="C79" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="D79" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1101</v>
       </c>
       <c r="E79" t="str">
-        <f>CHAR(A79)</f>
+        <f t="shared" si="8"/>
         <v>M</v>
       </c>
       <c r="F79" t="s">
         <v>38</v>
       </c>
       <c r="H79" s="5">
+        <f t="shared" si="12"/>
+        <v>12</v>
+      </c>
+      <c r="I79" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+        <v>CD</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>78</v>
       </c>
       <c r="B80" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4E</v>
       </c>
       <c r="C80" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="D80" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1110</v>
       </c>
       <c r="E80" t="str">
-        <f>CHAR(A80)</f>
+        <f t="shared" si="8"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>CE</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>79</v>
       </c>
       <c r="B81" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4F</v>
       </c>
       <c r="C81" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="D81" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1111</v>
       </c>
       <c r="E81" t="str">
-        <f>CHAR(A81)</f>
+        <f t="shared" si="8"/>
         <v>O</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>CF</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>80</v>
       </c>
       <c r="B82" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
       <c r="C82" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="D82" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0000</v>
       </c>
       <c r="E82" t="str">
-        <f>CHAR(A82)</f>
+        <f t="shared" si="8"/>
         <v>P</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>D0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>81</v>
       </c>
       <c r="B83" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>51</v>
       </c>
       <c r="C83" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="D83" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0001</v>
       </c>
       <c r="E83" t="str">
-        <f>CHAR(A83)</f>
+        <f t="shared" si="8"/>
         <v>Q</v>
       </c>
       <c r="F83" t="s">
         <v>39</v>
       </c>
       <c r="H83" s="5">
-        <f t="shared" ref="H83:H92" si="10">A83-65</f>
+        <f t="shared" ref="H83:H92" si="13">A83-65</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>D1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>82</v>
       </c>
       <c r="B84" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>52</v>
       </c>
       <c r="C84" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="D84" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0010</v>
       </c>
       <c r="E84" t="str">
-        <f>CHAR(A84)</f>
+        <f t="shared" si="8"/>
         <v>R</v>
       </c>
       <c r="F84" t="s">
         <v>40</v>
       </c>
       <c r="H84" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>D2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>83</v>
       </c>
       <c r="B85" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>53</v>
       </c>
       <c r="C85" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="D85" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0011</v>
       </c>
       <c r="E85" t="str">
-        <f>CHAR(A85)</f>
+        <f t="shared" si="8"/>
         <v>S</v>
       </c>
       <c r="F85" t="s">
         <v>41</v>
       </c>
       <c r="H85" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>D3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>84</v>
       </c>
       <c r="B86" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>54</v>
       </c>
       <c r="C86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="D86" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0100</v>
       </c>
       <c r="E86" t="str">
-        <f>CHAR(A86)</f>
+        <f t="shared" si="8"/>
         <v>T</v>
       </c>
       <c r="F86" t="s">
         <v>42</v>
       </c>
       <c r="H86" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>D4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>85</v>
       </c>
       <c r="B87" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>55</v>
       </c>
       <c r="C87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="D87" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0101</v>
       </c>
       <c r="E87" t="str">
-        <f>CHAR(A87)</f>
+        <f t="shared" si="8"/>
         <v>U</v>
       </c>
       <c r="F87" t="s">
         <v>43</v>
       </c>
       <c r="H87" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>D5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>86</v>
       </c>
       <c r="B88" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>56</v>
       </c>
       <c r="C88" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="D88" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0110</v>
       </c>
       <c r="E88" t="str">
-        <f>CHAR(A88)</f>
+        <f t="shared" si="8"/>
         <v>V</v>
       </c>
       <c r="F88" t="s">
         <v>44</v>
       </c>
       <c r="H88" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>D6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>87</v>
       </c>
       <c r="B89" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>57</v>
       </c>
       <c r="C89" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="D89" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0111</v>
       </c>
       <c r="E89" t="str">
-        <f>CHAR(A89)</f>
+        <f t="shared" si="8"/>
         <v>W</v>
       </c>
       <c r="F89" t="s">
         <v>45</v>
       </c>
       <c r="H89" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>D7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>88</v>
       </c>
       <c r="B90" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>58</v>
       </c>
       <c r="C90" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="D90" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1000</v>
       </c>
       <c r="E90" t="str">
-        <f>CHAR(A90)</f>
+        <f t="shared" si="8"/>
         <v>X</v>
       </c>
       <c r="F90" t="s">
         <v>46</v>
       </c>
       <c r="H90" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>D8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>89</v>
       </c>
       <c r="B91" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>59</v>
       </c>
       <c r="C91" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="D91" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1001</v>
       </c>
       <c r="E91" t="str">
-        <f>CHAR(A91)</f>
+        <f t="shared" si="8"/>
         <v>Y</v>
       </c>
       <c r="F91" t="s">
         <v>47</v>
       </c>
       <c r="H91" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>D9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>90</v>
       </c>
       <c r="B92" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5A</v>
       </c>
       <c r="C92" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="D92" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1010</v>
       </c>
       <c r="E92" t="str">
-        <f>CHAR(A92)</f>
+        <f t="shared" si="8"/>
         <v>Z</v>
       </c>
       <c r="F92" t="s">
         <v>48</v>
       </c>
       <c r="H92" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>DA</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>91</v>
       </c>
       <c r="B93" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5B</v>
       </c>
       <c r="C93" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="D93" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1011</v>
       </c>
       <c r="E93" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>DB</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>92</v>
       </c>
       <c r="B94" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5C</v>
       </c>
       <c r="C94" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="D94" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1100</v>
       </c>
       <c r="E94" t="s">
@@ -2901,22 +3026,26 @@
       <c r="F94" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>DC</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>93</v>
       </c>
       <c r="B95" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5D</v>
       </c>
       <c r="C95" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="D95" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1101</v>
       </c>
       <c r="E95" t="s">
@@ -2925,22 +3054,26 @@
       <c r="F95" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>DD</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>94</v>
       </c>
       <c r="B96" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5E</v>
       </c>
       <c r="C96" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="D96" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1110</v>
       </c>
       <c r="E96" t="s">
@@ -2949,22 +3082,26 @@
       <c r="F96" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I96" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>DE</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>95</v>
       </c>
       <c r="B97" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5F</v>
       </c>
       <c r="C97" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="D97" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1111</v>
       </c>
       <c r="E97" t="s">
@@ -2973,22 +3110,26 @@
       <c r="F97" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I97" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>DF</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>96</v>
       </c>
       <c r="B98" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
       <c r="C98" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="D98" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0000</v>
       </c>
       <c r="E98" t="s">
@@ -2998,350 +3139,350 @@
         <v>70</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>97</v>
       </c>
       <c r="B99" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>61</v>
       </c>
       <c r="C99" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="D99" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0001</v>
       </c>
       <c r="E99" t="str">
-        <f>CHAR(A99)</f>
+        <f t="shared" ref="E99:E124" si="14">CHAR(A99)</f>
         <v>a</v>
       </c>
       <c r="F99" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>98</v>
       </c>
       <c r="B100" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>62</v>
       </c>
       <c r="C100" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="D100" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0010</v>
       </c>
       <c r="E100" t="str">
-        <f>CHAR(A100)</f>
+        <f t="shared" si="14"/>
         <v>b</v>
       </c>
       <c r="F100" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>99</v>
       </c>
       <c r="B101" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>63</v>
       </c>
       <c r="C101" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="D101" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0011</v>
       </c>
       <c r="E101" t="str">
-        <f>CHAR(A101)</f>
+        <f t="shared" si="14"/>
         <v>c</v>
       </c>
       <c r="F101" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
       <c r="B102" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>64</v>
       </c>
       <c r="C102" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="D102" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0100</v>
       </c>
       <c r="E102" t="str">
-        <f>CHAR(A102)</f>
+        <f t="shared" si="14"/>
         <v>d</v>
       </c>
       <c r="F102" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>101</v>
       </c>
       <c r="B103" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65</v>
       </c>
       <c r="C103" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="D103" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0101</v>
       </c>
       <c r="E103" t="str">
-        <f>CHAR(A103)</f>
+        <f t="shared" si="14"/>
         <v>e</v>
       </c>
       <c r="F103" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>102</v>
       </c>
       <c r="B104" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>66</v>
       </c>
       <c r="C104" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="D104" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0110</v>
       </c>
       <c r="E104" t="str">
-        <f>CHAR(A104)</f>
+        <f t="shared" si="14"/>
         <v>f</v>
       </c>
       <c r="F104" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>103</v>
       </c>
       <c r="B105" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>67</v>
       </c>
       <c r="C105" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="D105" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0111</v>
       </c>
       <c r="E105" t="str">
-        <f>CHAR(A105)</f>
+        <f t="shared" si="14"/>
         <v>g</v>
       </c>
       <c r="F105" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>104</v>
       </c>
       <c r="B106" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>68</v>
       </c>
       <c r="C106" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="D106" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1000</v>
       </c>
       <c r="E106" t="str">
-        <f>CHAR(A106)</f>
+        <f t="shared" si="14"/>
         <v>h</v>
       </c>
       <c r="F106" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>105</v>
       </c>
       <c r="B107" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>69</v>
       </c>
       <c r="C107" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="D107" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1001</v>
       </c>
       <c r="E107" t="str">
-        <f>CHAR(A107)</f>
+        <f t="shared" si="14"/>
         <v>i</v>
       </c>
       <c r="F107" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>106</v>
       </c>
       <c r="B108" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6A</v>
       </c>
       <c r="C108" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="D108" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1010</v>
       </c>
       <c r="E108" t="str">
-        <f>CHAR(A108)</f>
+        <f t="shared" si="14"/>
         <v>j</v>
       </c>
       <c r="F108" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>107</v>
       </c>
       <c r="B109" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6B</v>
       </c>
       <c r="C109" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="D109" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1011</v>
       </c>
       <c r="E109" t="str">
-        <f>CHAR(A109)</f>
+        <f t="shared" si="14"/>
         <v>k</v>
       </c>
       <c r="F109" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>108</v>
       </c>
       <c r="B110" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6C</v>
       </c>
       <c r="C110" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="D110" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1100</v>
       </c>
       <c r="E110" t="str">
-        <f>CHAR(A110)</f>
+        <f t="shared" si="14"/>
         <v>l</v>
       </c>
       <c r="F110" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>109</v>
       </c>
       <c r="B111" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6D</v>
       </c>
       <c r="C111" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="D111" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1101</v>
       </c>
       <c r="E111" t="str">
-        <f>CHAR(A111)</f>
+        <f t="shared" si="14"/>
         <v>m</v>
       </c>
       <c r="F111" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>110</v>
       </c>
       <c r="B112" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6E</v>
       </c>
       <c r="C112" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="D112" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1110</v>
       </c>
       <c r="E112" t="str">
-        <f>CHAR(A112)</f>
+        <f t="shared" si="14"/>
         <v>n</v>
       </c>
       <c r="F112" t="s">
@@ -3350,23 +3491,23 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>111</v>
       </c>
       <c r="B113" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6F</v>
       </c>
       <c r="C113" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="D113" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1111</v>
       </c>
       <c r="E113" t="str">
-        <f>CHAR(A113)</f>
+        <f t="shared" si="14"/>
         <v>o</v>
       </c>
       <c r="F113" t="s">
@@ -3375,23 +3516,23 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>112</v>
       </c>
       <c r="B114" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>70</v>
       </c>
       <c r="C114" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
       <c r="D114" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0000</v>
       </c>
       <c r="E114" t="str">
-        <f>CHAR(A114)</f>
+        <f t="shared" si="14"/>
         <v>p</v>
       </c>
       <c r="F114" t="s">
@@ -3400,23 +3541,23 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>113</v>
       </c>
       <c r="B115" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>71</v>
       </c>
       <c r="C115" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
       <c r="D115" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0001</v>
       </c>
       <c r="E115" t="str">
-        <f>CHAR(A115)</f>
+        <f t="shared" si="14"/>
         <v>q</v>
       </c>
       <c r="F115" t="s">
@@ -3425,23 +3566,23 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>114</v>
       </c>
       <c r="B116" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72</v>
       </c>
       <c r="C116" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
       <c r="D116" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0010</v>
       </c>
       <c r="E116" t="str">
-        <f>CHAR(A116)</f>
+        <f t="shared" si="14"/>
         <v>r</v>
       </c>
       <c r="F116" t="s">
@@ -3450,23 +3591,23 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>115</v>
       </c>
       <c r="B117" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>73</v>
       </c>
       <c r="C117" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
       <c r="D117" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0011</v>
       </c>
       <c r="E117" t="str">
-        <f>CHAR(A117)</f>
+        <f t="shared" si="14"/>
         <v>s</v>
       </c>
       <c r="F117" t="s">
@@ -3475,23 +3616,23 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>116</v>
       </c>
       <c r="B118" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74</v>
       </c>
       <c r="C118" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
       <c r="D118" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0100</v>
       </c>
       <c r="E118" t="str">
-        <f>CHAR(A118)</f>
+        <f t="shared" si="14"/>
         <v>t</v>
       </c>
       <c r="F118" t="s">
@@ -3500,23 +3641,23 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>117</v>
       </c>
       <c r="B119" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
       <c r="C119" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
       <c r="D119" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0101</v>
       </c>
       <c r="E119" t="str">
-        <f>CHAR(A119)</f>
+        <f t="shared" si="14"/>
         <v>u</v>
       </c>
       <c r="F119" t="s">
@@ -3525,23 +3666,23 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>118</v>
       </c>
       <c r="B120" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>76</v>
       </c>
       <c r="C120" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
       <c r="D120" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0110</v>
       </c>
       <c r="E120" t="str">
-        <f>CHAR(A120)</f>
+        <f t="shared" si="14"/>
         <v>v</v>
       </c>
       <c r="F120" t="s">
@@ -3550,23 +3691,23 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>119</v>
       </c>
       <c r="B121" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>77</v>
       </c>
       <c r="C121" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
       <c r="D121" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0111</v>
       </c>
       <c r="E121" t="str">
-        <f>CHAR(A121)</f>
+        <f t="shared" si="14"/>
         <v>w</v>
       </c>
       <c r="F121" t="s">
@@ -3575,23 +3716,23 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>120</v>
       </c>
       <c r="B122" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>78</v>
       </c>
       <c r="C122" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
       <c r="D122" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1000</v>
       </c>
       <c r="E122" t="str">
-        <f>CHAR(A122)</f>
+        <f t="shared" si="14"/>
         <v>x</v>
       </c>
       <c r="F122" t="s">
@@ -3600,23 +3741,23 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>121</v>
       </c>
       <c r="B123" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>79</v>
       </c>
       <c r="C123" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
       <c r="D123" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1001</v>
       </c>
       <c r="E123" t="str">
-        <f>CHAR(A123)</f>
+        <f t="shared" si="14"/>
         <v>y</v>
       </c>
       <c r="F123" t="s">
@@ -3625,23 +3766,23 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>122</v>
       </c>
       <c r="B124" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7A</v>
       </c>
       <c r="C124" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
       <c r="D124" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1010</v>
       </c>
       <c r="E124" t="str">
-        <f>CHAR(A124)</f>
+        <f t="shared" si="14"/>
         <v>z</v>
       </c>
       <c r="F124" t="s">
@@ -3650,19 +3791,19 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>123</v>
       </c>
       <c r="B125" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7B</v>
       </c>
       <c r="C125" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
       <c r="D125" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1011</v>
       </c>
       <c r="E125" t="s">
@@ -3674,19 +3815,19 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>124</v>
       </c>
       <c r="B126" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7C</v>
       </c>
       <c r="C126" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
       <c r="D126" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1100</v>
       </c>
       <c r="E126" t="s">
@@ -3698,19 +3839,19 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>125</v>
       </c>
       <c r="B127" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7D</v>
       </c>
       <c r="C127" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
       <c r="D127" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1101</v>
       </c>
       <c r="E127" t="s">
@@ -3722,19 +3863,19 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>126</v>
       </c>
       <c r="B128" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7E</v>
       </c>
       <c r="C128" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
       <c r="D128" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1110</v>
       </c>
       <c r="E128" t="s">
@@ -3746,19 +3887,19 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>127</v>
       </c>
       <c r="B129" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7F</v>
       </c>
       <c r="C129" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
       <c r="D129" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1111</v>
       </c>
       <c r="E129" t="s">

</xml_diff>

<commit_message>
Added NXtelMonitor project which can kill servers, and send messages to the page manager to restart them. Servers can now be disabled and enabled in teh page manager.
</commit_message>
<xml_diff>
--- a/docs/prestel character set.xlsx
+++ b/docs/prestel character set.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\Visual Studio 2015\Projects\NXtel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13241AC8-83F2-46C7-B1ED-C0FA1A48B57C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FF5A3A-6AC4-4947-B606-4CE23C3D3653}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" xr2:uid="{4E45CEFB-9C71-41FA-8F36-CA32F2ADC803}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -634,8 +636,8 @@
   <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K95" sqref="K95"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3913,4 +3915,1084 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C81DD96-316C-4402-8D42-84A4FD3618FC}">
+  <dimension ref="A1:D105"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <f xml:space="preserve"> INT(A1/8)</f>
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <f>5*24</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>A1+1</f>
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B65" si="0" xml:space="preserve"> INT(A2/8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A42" si="1">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f>A37+1</f>
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" ref="A43:A105" si="2">A42+1</f>
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <f t="shared" ref="B66:B105" si="3" xml:space="preserve"> INT(A66/8)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <f t="shared" si="2"/>
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <f t="shared" si="2"/>
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" si="2"/>
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <f t="shared" si="2"/>
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <f t="shared" si="2"/>
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <f t="shared" si="2"/>
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <f t="shared" si="2"/>
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <f t="shared" si="2"/>
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <f t="shared" si="2"/>
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <f t="shared" si="2"/>
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <f t="shared" si="2"/>
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <f t="shared" si="2"/>
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <f t="shared" si="2"/>
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <f t="shared" si="2"/>
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <f t="shared" si="2"/>
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <f t="shared" si="2"/>
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <f t="shared" si="2"/>
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <f t="shared" si="2"/>
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <f t="shared" si="2"/>
+        <v>101</v>
+      </c>
+      <c r="B102">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <f t="shared" si="2"/>
+        <v>102</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <f t="shared" si="2"/>
+        <v>103</v>
+      </c>
+      <c r="B104">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <f t="shared" si="2"/>
+        <v>104</v>
+      </c>
+      <c r="B105">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E4F66D-3A10-44F9-BF79-FCCAF365461F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Server prints options when starting up. Tidied up page manager account creation, including error handling. Page manager can handle users with blank mailboxes.
</commit_message>
<xml_diff>
--- a/docs/prestel character set.xlsx
+++ b/docs/prestel character set.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\Visual Studio 2015\Projects\NXtel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FF5A3A-6AC4-4947-B606-4CE23C3D3653}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F580A16C-6D1A-440C-8916-6CA4F03ACBF8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" xr2:uid="{4E45CEFB-9C71-41FA-8F36-CA32F2ADC803}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" activeTab="3" xr2:uid="{4E45CEFB-9C71-41FA-8F36-CA32F2ADC803}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="77">
   <si>
     <t>ASCII</t>
   </si>
@@ -255,6 +256,15 @@
   </si>
   <si>
     <t>Shifted</t>
+  </si>
+  <si>
+    <t>A108</t>
+  </si>
+  <si>
+    <t>A908</t>
+  </si>
+  <si>
+    <t>B108</t>
   </si>
 </sst>
 </file>
@@ -635,7 +645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FEC36D4-E8A2-4FCB-BFF9-8DA7DDB6CAE4}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
@@ -4995,4 +5005,391 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7FAD3BD-5010-4E98-857F-3E3E6C529092}">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.140625" style="7"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <f>A1*8</f>
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="str">
+        <f>DEC2HEX(B1, 2)</f>
+        <v>00</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>A1+1</f>
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B24" si="0">A2*8</f>
+        <v>8</v>
+      </c>
+      <c r="C2" s="7" t="str">
+        <f t="shared" ref="C2:C24" si="1">DEC2HEX(B2, 2)</f>
+        <v>08</v>
+      </c>
+      <c r="E2" s="1">
+        <v>6908</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f t="shared" ref="A3:A24" si="2">A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C3" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="E3" s="1">
+        <v>7108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C4" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="E4" s="1">
+        <v>7908</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="C5" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="E5" s="1">
+        <v>8108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="C6" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="E6" s="1">
+        <v>8908</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="C7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="E7" s="1">
+        <v>9108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="C8" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="E8" s="1">
+        <v>9908</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="C9" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="C10" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="C11" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="C12" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="C13" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+      <c r="C14" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="C15" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="C16" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="C17" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f>A17+1</f>
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>136</v>
+      </c>
+      <c r="C18" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="C19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>152</v>
+      </c>
+      <c r="C20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="C21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>A0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>168</v>
+      </c>
+      <c r="C22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>A8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f>A22+1</f>
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>176</v>
+      </c>
+      <c r="C23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>B0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>184</v>
+      </c>
+      <c r="C24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>B8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Server now accommodates "deferred CRLF" mode in the Telstar BBC BASIC SDL client. Any completely blank lines immediately following a non-trimmed wrapping line now contain a 0x09 before the CRLF on the blank line.
</commit_message>
<xml_diff>
--- a/docs/prestel character set.xlsx
+++ b/docs/prestel character set.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\Visual Studio 2015\Projects\NXtel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F580A16C-6D1A-440C-8916-6CA4F03ACBF8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0D7FA8-B6E9-4733-87F8-A74B8A7F6A4E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" activeTab="3" xr2:uid="{4E45CEFB-9C71-41FA-8F36-CA32F2ADC803}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{4E45CEFB-9C71-41FA-8F36-CA32F2ADC803}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Prestel" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="74">
   <si>
     <t>ASCII</t>
   </si>
@@ -256,15 +253,6 @@
   </si>
   <si>
     <t>Shifted</t>
-  </si>
-  <si>
-    <t>A108</t>
-  </si>
-  <si>
-    <t>A908</t>
-  </si>
-  <si>
-    <t>B108</t>
   </si>
 </sst>
 </file>
@@ -645,9 +633,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FEC36D4-E8A2-4FCB-BFF9-8DA7DDB6CAE4}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3925,1471 +3913,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C81DD96-316C-4402-8D42-84A4FD3618FC}">
-  <dimension ref="A1:D105"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <f xml:space="preserve"> INT(A1/8)</f>
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <f>5*24</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f>A1+1</f>
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <f t="shared" ref="B2:B65" si="0" xml:space="preserve"> INT(A2/8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f>A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f t="shared" ref="A4:A42" si="1">A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="B36">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="B37">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <f>A37+1</f>
-        <v>37</v>
-      </c>
-      <c r="B38">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="B39">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <f t="shared" si="1"/>
-        <v>39</v>
-      </c>
-      <c r="B40">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="B41">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="B42">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <f t="shared" ref="A43:A105" si="2">A42+1</f>
-        <v>42</v>
-      </c>
-      <c r="B43">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <f t="shared" si="2"/>
-        <v>43</v>
-      </c>
-      <c r="B44">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="B45">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <f t="shared" si="2"/>
-        <v>45</v>
-      </c>
-      <c r="B46">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <f t="shared" si="2"/>
-        <v>46</v>
-      </c>
-      <c r="B47">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <f t="shared" si="2"/>
-        <v>47</v>
-      </c>
-      <c r="B48">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <f t="shared" si="2"/>
-        <v>48</v>
-      </c>
-      <c r="B49">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <f t="shared" si="2"/>
-        <v>49</v>
-      </c>
-      <c r="B50">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="B51">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <f t="shared" si="2"/>
-        <v>51</v>
-      </c>
-      <c r="B52">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <f t="shared" si="2"/>
-        <v>52</v>
-      </c>
-      <c r="B53">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <f t="shared" si="2"/>
-        <v>53</v>
-      </c>
-      <c r="B54">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <f t="shared" si="2"/>
-        <v>54</v>
-      </c>
-      <c r="B55">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <f t="shared" si="2"/>
-        <v>55</v>
-      </c>
-      <c r="B56">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <f t="shared" si="2"/>
-        <v>56</v>
-      </c>
-      <c r="B57">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <f t="shared" si="2"/>
-        <v>57</v>
-      </c>
-      <c r="B58">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <f t="shared" si="2"/>
-        <v>58</v>
-      </c>
-      <c r="B59">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <f t="shared" si="2"/>
-        <v>59</v>
-      </c>
-      <c r="B60">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="B61">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <f t="shared" si="2"/>
-        <v>61</v>
-      </c>
-      <c r="B62">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <f t="shared" si="2"/>
-        <v>62</v>
-      </c>
-      <c r="B63">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <f t="shared" si="2"/>
-        <v>63</v>
-      </c>
-      <c r="B64">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <f t="shared" si="2"/>
-        <v>64</v>
-      </c>
-      <c r="B65">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <f t="shared" si="2"/>
-        <v>65</v>
-      </c>
-      <c r="B66">
-        <f t="shared" ref="B66:B105" si="3" xml:space="preserve"> INT(A66/8)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <f t="shared" si="2"/>
-        <v>66</v>
-      </c>
-      <c r="B67">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <f t="shared" si="2"/>
-        <v>67</v>
-      </c>
-      <c r="B68">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <f t="shared" si="2"/>
-        <v>68</v>
-      </c>
-      <c r="B69">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <f t="shared" si="2"/>
-        <v>69</v>
-      </c>
-      <c r="B70">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="B71">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <f t="shared" si="2"/>
-        <v>71</v>
-      </c>
-      <c r="B72">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <f t="shared" si="2"/>
-        <v>72</v>
-      </c>
-      <c r="B73">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <f t="shared" si="2"/>
-        <v>73</v>
-      </c>
-      <c r="B74">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <f t="shared" si="2"/>
-        <v>74</v>
-      </c>
-      <c r="B75">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <f t="shared" si="2"/>
-        <v>75</v>
-      </c>
-      <c r="B76">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <f t="shared" si="2"/>
-        <v>76</v>
-      </c>
-      <c r="B77">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <f t="shared" si="2"/>
-        <v>77</v>
-      </c>
-      <c r="B78">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <f t="shared" si="2"/>
-        <v>78</v>
-      </c>
-      <c r="B79">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <f t="shared" si="2"/>
-        <v>79</v>
-      </c>
-      <c r="B80">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <f t="shared" si="2"/>
-        <v>80</v>
-      </c>
-      <c r="B81">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <f t="shared" si="2"/>
-        <v>81</v>
-      </c>
-      <c r="B82">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <f t="shared" si="2"/>
-        <v>82</v>
-      </c>
-      <c r="B83">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <f t="shared" si="2"/>
-        <v>83</v>
-      </c>
-      <c r="B84">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <f t="shared" si="2"/>
-        <v>84</v>
-      </c>
-      <c r="B85">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <f t="shared" si="2"/>
-        <v>85</v>
-      </c>
-      <c r="B86">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <f t="shared" si="2"/>
-        <v>86</v>
-      </c>
-      <c r="B87">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <f t="shared" si="2"/>
-        <v>87</v>
-      </c>
-      <c r="B88">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <f t="shared" si="2"/>
-        <v>88</v>
-      </c>
-      <c r="B89">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <f t="shared" si="2"/>
-        <v>89</v>
-      </c>
-      <c r="B90">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <f t="shared" si="2"/>
-        <v>90</v>
-      </c>
-      <c r="B91">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <f t="shared" si="2"/>
-        <v>91</v>
-      </c>
-      <c r="B92">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <f t="shared" si="2"/>
-        <v>92</v>
-      </c>
-      <c r="B93">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <f t="shared" si="2"/>
-        <v>93</v>
-      </c>
-      <c r="B94">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <f t="shared" si="2"/>
-        <v>94</v>
-      </c>
-      <c r="B95">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <f t="shared" si="2"/>
-        <v>95</v>
-      </c>
-      <c r="B96">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <f t="shared" si="2"/>
-        <v>96</v>
-      </c>
-      <c r="B97">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <f t="shared" si="2"/>
-        <v>97</v>
-      </c>
-      <c r="B98">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-      <c r="B99">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <f t="shared" si="2"/>
-        <v>99</v>
-      </c>
-      <c r="B100">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="B101">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102">
-        <f t="shared" si="2"/>
-        <v>101</v>
-      </c>
-      <c r="B102">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103">
-        <f t="shared" si="2"/>
-        <v>102</v>
-      </c>
-      <c r="B103">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104">
-        <f t="shared" si="2"/>
-        <v>103</v>
-      </c>
-      <c r="B104">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105">
-        <f t="shared" si="2"/>
-        <v>104</v>
-      </c>
-      <c r="B105">
-        <f t="shared" si="3"/>
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E4F66D-3A10-44F9-BF79-FCCAF365461F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7FAD3BD-5010-4E98-857F-3E3E6C529092}">
-  <dimension ref="A1:E24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="9.140625" style="7"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <f>A1*8</f>
-        <v>0</v>
-      </c>
-      <c r="C1" s="7" t="str">
-        <f>DEC2HEX(B1, 2)</f>
-        <v>00</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f>A1+1</f>
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <f t="shared" ref="B2:B24" si="0">A2*8</f>
-        <v>8</v>
-      </c>
-      <c r="C2" s="7" t="str">
-        <f t="shared" ref="C2:C24" si="1">DEC2HEX(B2, 2)</f>
-        <v>08</v>
-      </c>
-      <c r="E2" s="1">
-        <v>6908</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f t="shared" ref="A3:A24" si="2">A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="C3" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="E3" s="1">
-        <v>7108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="C4" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="E4" s="1">
-        <v>7908</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="C5" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="E5" s="1">
-        <v>8108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="C6" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="E6" s="1">
-        <v>8908</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="C7" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="E7" s="1">
-        <v>9108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="C8" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="E8" s="1">
-        <v>9908</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="C9" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="C10" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="C11" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-      <c r="C12" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>96</v>
-      </c>
-      <c r="C13" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>104</v>
-      </c>
-      <c r="C14" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>112</v>
-      </c>
-      <c r="C15" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="C16" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>128</v>
-      </c>
-      <c r="C17" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f>A17+1</f>
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>136</v>
-      </c>
-      <c r="C18" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>144</v>
-      </c>
-      <c r="C19" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>152</v>
-      </c>
-      <c r="C20" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>160</v>
-      </c>
-      <c r="C21" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>A0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>168</v>
-      </c>
-      <c r="C22" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>A8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f>A22+1</f>
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <f t="shared" si="0"/>
-        <v>176</v>
-      </c>
-      <c r="C23" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>B0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <f t="shared" si="0"/>
-        <v>184</v>
-      </c>
-      <c r="C24" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>B8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Page rendering now sets flags for every line with a double-height code. The double-height fill-below routine checks this flag and skips the fill if the line is single height. This lets partial overprinting work without blanking out the line below the overprinted line.
</commit_message>
<xml_diff>
--- a/docs/prestel character set.xlsx
+++ b/docs/prestel character set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\Visual Studio 2015\Projects\NXtel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0D7FA8-B6E9-4733-87F8-A74B8A7F6A4E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8985B54D-5FAC-467E-9D18-8599F725D815}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{4E45CEFB-9C71-41FA-8F36-CA32F2ADC803}"/>
   </bookViews>
@@ -634,8 +634,8 @@
   <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q71" sqref="Q71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2180,8 +2180,8 @@
         <v>28</v>
       </c>
       <c r="H67" s="5">
-        <f>A67-65</f>
-        <v>0</v>
+        <f>A67-64</f>
+        <v>1</v>
       </c>
       <c r="I67" s="7" t="str">
         <f t="shared" ref="I67:I97" si="9">DEC2HEX(A67+128, 2)</f>
@@ -2213,8 +2213,8 @@
         <v>29</v>
       </c>
       <c r="H68" s="5">
-        <f t="shared" ref="H68:H75" si="11">A68-65</f>
-        <v>1</v>
+        <f t="shared" ref="H68:H75" si="11">A68-64</f>
+        <v>2</v>
       </c>
       <c r="I68" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="H69" s="5">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I69" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2280,7 +2280,7 @@
       </c>
       <c r="H70" s="5">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I70" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2313,7 +2313,7 @@
       </c>
       <c r="H71" s="5">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I71" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="H72" s="5">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I72" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2379,7 +2379,7 @@
       </c>
       <c r="H73" s="5">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I73" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="H74" s="5">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I74" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="H75" s="5">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I75" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2529,8 +2529,8 @@
         <v>37</v>
       </c>
       <c r="H78" s="5">
-        <f t="shared" ref="H78:H79" si="12">A78-65</f>
-        <v>11</v>
+        <f>A78-64</f>
+        <v>12</v>
       </c>
       <c r="I78" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2562,8 +2562,8 @@
         <v>38</v>
       </c>
       <c r="H79" s="5">
-        <f t="shared" si="12"/>
-        <v>12</v>
+        <f>A79-64</f>
+        <v>13</v>
       </c>
       <c r="I79" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2673,8 +2673,8 @@
         <v>39</v>
       </c>
       <c r="H83" s="5">
-        <f t="shared" ref="H83:H92" si="13">A83-65</f>
-        <v>16</v>
+        <f>A83-64</f>
+        <v>17</v>
       </c>
       <c r="I83" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2706,8 +2706,8 @@
         <v>40</v>
       </c>
       <c r="H84" s="5">
-        <f t="shared" si="13"/>
-        <v>17</v>
+        <f t="shared" ref="H84:H97" si="12">A84-64</f>
+        <v>18</v>
       </c>
       <c r="I84" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2739,8 +2739,8 @@
         <v>41</v>
       </c>
       <c r="H85" s="5">
-        <f t="shared" si="13"/>
-        <v>18</v>
+        <f t="shared" si="12"/>
+        <v>19</v>
       </c>
       <c r="I85" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2772,8 +2772,8 @@
         <v>42</v>
       </c>
       <c r="H86" s="5">
-        <f t="shared" si="13"/>
-        <v>19</v>
+        <f t="shared" si="12"/>
+        <v>20</v>
       </c>
       <c r="I86" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2805,8 +2805,8 @@
         <v>43</v>
       </c>
       <c r="H87" s="5">
-        <f t="shared" si="13"/>
-        <v>20</v>
+        <f t="shared" si="12"/>
+        <v>21</v>
       </c>
       <c r="I87" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2838,8 +2838,8 @@
         <v>44</v>
       </c>
       <c r="H88" s="5">
-        <f t="shared" si="13"/>
-        <v>21</v>
+        <f t="shared" si="12"/>
+        <v>22</v>
       </c>
       <c r="I88" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2871,8 +2871,8 @@
         <v>45</v>
       </c>
       <c r="H89" s="5">
-        <f t="shared" si="13"/>
-        <v>22</v>
+        <f t="shared" si="12"/>
+        <v>23</v>
       </c>
       <c r="I89" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2904,8 +2904,8 @@
         <v>46</v>
       </c>
       <c r="H90" s="5">
-        <f t="shared" si="13"/>
-        <v>23</v>
+        <f t="shared" si="12"/>
+        <v>24</v>
       </c>
       <c r="I90" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2937,8 +2937,8 @@
         <v>47</v>
       </c>
       <c r="H91" s="5">
-        <f t="shared" si="13"/>
-        <v>24</v>
+        <f t="shared" si="12"/>
+        <v>25</v>
       </c>
       <c r="I91" s="7" t="str">
         <f t="shared" si="9"/>
@@ -2970,8 +2970,8 @@
         <v>48</v>
       </c>
       <c r="H92" s="5">
-        <f t="shared" si="13"/>
-        <v>25</v>
+        <f t="shared" si="12"/>
+        <v>26</v>
       </c>
       <c r="I92" s="7" t="str">
         <f t="shared" si="9"/>
@@ -3026,6 +3026,10 @@
       <c r="F94" t="s">
         <v>49</v>
       </c>
+      <c r="H94" s="5">
+        <f t="shared" si="12"/>
+        <v>28</v>
+      </c>
       <c r="I94" s="7" t="str">
         <f t="shared" si="9"/>
         <v>DC</v>
@@ -3054,6 +3058,10 @@
       <c r="F95" t="s">
         <v>50</v>
       </c>
+      <c r="H95" s="5">
+        <f t="shared" si="12"/>
+        <v>29</v>
+      </c>
       <c r="I95" s="7" t="str">
         <f t="shared" si="9"/>
         <v>DD</v>
@@ -3082,6 +3090,10 @@
       <c r="F96" t="s">
         <v>51</v>
       </c>
+      <c r="H96" s="5">
+        <f t="shared" si="12"/>
+        <v>30</v>
+      </c>
       <c r="I96" s="7" t="str">
         <f t="shared" si="9"/>
         <v>DE</v>
@@ -3110,6 +3122,10 @@
       <c r="F97" t="s">
         <v>52</v>
       </c>
+      <c r="H97" s="5">
+        <f t="shared" si="12"/>
+        <v>31</v>
+      </c>
       <c r="I97" s="7" t="str">
         <f t="shared" si="9"/>
         <v>DF</v>
@@ -3157,7 +3173,7 @@
         <v>0001</v>
       </c>
       <c r="E99" t="str">
-        <f t="shared" ref="E99:E124" si="14">CHAR(A99)</f>
+        <f t="shared" ref="E99:E124" si="13">CHAR(A99)</f>
         <v>a</v>
       </c>
       <c r="F99" t="s">
@@ -3182,7 +3198,7 @@
         <v>0010</v>
       </c>
       <c r="E100" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>b</v>
       </c>
       <c r="F100" t="s">
@@ -3207,7 +3223,7 @@
         <v>0011</v>
       </c>
       <c r="E101" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>c</v>
       </c>
       <c r="F101" t="s">
@@ -3232,7 +3248,7 @@
         <v>0100</v>
       </c>
       <c r="E102" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>d</v>
       </c>
       <c r="F102" t="s">
@@ -3257,7 +3273,7 @@
         <v>0101</v>
       </c>
       <c r="E103" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>e</v>
       </c>
       <c r="F103" t="s">
@@ -3282,7 +3298,7 @@
         <v>0110</v>
       </c>
       <c r="E104" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>f</v>
       </c>
       <c r="F104" t="s">
@@ -3307,7 +3323,7 @@
         <v>0111</v>
       </c>
       <c r="E105" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>g</v>
       </c>
       <c r="F105" t="s">
@@ -3332,7 +3348,7 @@
         <v>1000</v>
       </c>
       <c r="E106" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>h</v>
       </c>
       <c r="F106" t="s">
@@ -3357,7 +3373,7 @@
         <v>1001</v>
       </c>
       <c r="E107" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>i</v>
       </c>
       <c r="F107" t="s">
@@ -3382,7 +3398,7 @@
         <v>1010</v>
       </c>
       <c r="E108" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>j</v>
       </c>
       <c r="F108" t="s">
@@ -3407,7 +3423,7 @@
         <v>1011</v>
       </c>
       <c r="E109" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>k</v>
       </c>
       <c r="F109" t="s">
@@ -3432,7 +3448,7 @@
         <v>1100</v>
       </c>
       <c r="E110" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>l</v>
       </c>
       <c r="F110" t="s">
@@ -3457,7 +3473,7 @@
         <v>1101</v>
       </c>
       <c r="E111" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>m</v>
       </c>
       <c r="F111" t="s">
@@ -3482,7 +3498,7 @@
         <v>1110</v>
       </c>
       <c r="E112" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>n</v>
       </c>
       <c r="F112" t="s">
@@ -3507,7 +3523,7 @@
         <v>1111</v>
       </c>
       <c r="E113" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>o</v>
       </c>
       <c r="F113" t="s">
@@ -3532,7 +3548,7 @@
         <v>0000</v>
       </c>
       <c r="E114" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>p</v>
       </c>
       <c r="F114" t="s">
@@ -3557,7 +3573,7 @@
         <v>0001</v>
       </c>
       <c r="E115" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>q</v>
       </c>
       <c r="F115" t="s">
@@ -3582,7 +3598,7 @@
         <v>0010</v>
       </c>
       <c r="E116" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>r</v>
       </c>
       <c r="F116" t="s">
@@ -3607,7 +3623,7 @@
         <v>0011</v>
       </c>
       <c r="E117" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>s</v>
       </c>
       <c r="F117" t="s">
@@ -3632,7 +3648,7 @@
         <v>0100</v>
       </c>
       <c r="E118" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>t</v>
       </c>
       <c r="F118" t="s">
@@ -3657,7 +3673,7 @@
         <v>0101</v>
       </c>
       <c r="E119" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>u</v>
       </c>
       <c r="F119" t="s">
@@ -3682,7 +3698,7 @@
         <v>0110</v>
       </c>
       <c r="E120" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>v</v>
       </c>
       <c r="F120" t="s">
@@ -3707,7 +3723,7 @@
         <v>0111</v>
       </c>
       <c r="E121" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>w</v>
       </c>
       <c r="F121" t="s">
@@ -3732,7 +3748,7 @@
         <v>1000</v>
       </c>
       <c r="E122" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>x</v>
       </c>
       <c r="F122" t="s">
@@ -3757,7 +3773,7 @@
         <v>1001</v>
       </c>
       <c r="E123" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>y</v>
       </c>
       <c r="F123" t="s">
@@ -3782,7 +3798,7 @@
         <v>1010</v>
       </c>
       <c r="E124" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>z</v>
       </c>
       <c r="F124" t="s">

</xml_diff>